<commit_message>
Updated excel for week2
</commit_message>
<xml_diff>
--- a/Project Allocation.xlsx
+++ b/Project Allocation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Project Name</t>
   </si>
@@ -46,15 +46,9 @@
     <t>Register page front + back</t>
   </si>
   <si>
-    <t>Dashboard user front + back</t>
-  </si>
-  <si>
     <t>Login page frontend, navbar</t>
   </si>
   <si>
-    <t>Dashboard administrator front + back, login backend</t>
-  </si>
-  <si>
     <t>7 zile</t>
   </si>
   <si>
@@ -80,13 +74,28 @@
   </si>
   <si>
     <t>Polls admin</t>
+  </si>
+  <si>
+    <t>Invoices user front + back</t>
+  </si>
+  <si>
+    <t>Week1</t>
+  </si>
+  <si>
+    <t>Week2</t>
+  </si>
+  <si>
+    <t>Login front + back, routing and login protection</t>
+  </si>
+  <si>
+    <t>Dashboard administrator front + back</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -106,6 +115,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,11 +150,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,10 +372,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -361,7 +385,7 @@
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -369,7 +393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -380,91 +404,124 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
+    <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>15</v>
+      <c r="A9" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>16</v>
+      <c r="A10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
+      <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
+      <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>